<commit_message>
Add first 19 users
</commit_message>
<xml_diff>
--- a/users-list.xlsx
+++ b/users-list.xlsx
@@ -19,31 +19,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>huconnectedtest-00001</t>
-  </si>
-  <si>
-    <t>huconnectedtest-00002</t>
-  </si>
-  <si>
-    <t>huconnectedtest-00003</t>
-  </si>
-  <si>
-    <t>huconnectedtest-00004</t>
-  </si>
-  <si>
-    <t>huconnectedtest-00005</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+  <si>
+    <t>huconnected0026</t>
+  </si>
+  <si>
+    <t>huconnected0058</t>
+  </si>
+  <si>
+    <t>huconnected0059</t>
+  </si>
+  <si>
+    <t>huconnected0036</t>
+  </si>
+  <si>
+    <t>huconnected0027</t>
+  </si>
+  <si>
+    <t>huconnected0005</t>
+  </si>
+  <si>
+    <t>huconnected0006</t>
+  </si>
+  <si>
+    <t>huconnected0007</t>
+  </si>
+  <si>
+    <t>huconnected0008</t>
+  </si>
+  <si>
+    <t>huconnected0009</t>
+  </si>
+  <si>
+    <t>huconnected0010</t>
+  </si>
+  <si>
+    <t>huconnected0011</t>
+  </si>
+  <si>
+    <t>huconnected0012</t>
+  </si>
+  <si>
+    <t>huconnected0013</t>
+  </si>
+  <si>
+    <t>huconnected0014</t>
+  </si>
+  <si>
+    <t>huconnected0015</t>
+  </si>
+  <si>
+    <t>huconnected0016</t>
+  </si>
+  <si>
+    <t>huconnected0046</t>
+  </si>
+  <si>
+    <t>huconnected0085</t>
+  </si>
+  <si>
+    <t>2023-04-26</t>
+  </si>
+  <si>
+    <t>2023-05-06</t>
+  </si>
+  <si>
+    <t>2023-05-02</t>
+  </si>
+  <si>
+    <t>2023-05-04</t>
+  </si>
+  <si>
+    <t>2023-05-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,12 +113,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,17 +136,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,43 +446,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>